<commit_message>
FB validation bug fixed
</commit_message>
<xml_diff>
--- a/admin/uploads/excel.xlsx
+++ b/admin/uploads/excel.xlsx
@@ -301,13 +301,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>287267</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1253636</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>874783</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -315,7 +315,7 @@
         <xdr:cNvPr id="5" name="Picture 4" descr="test image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AB1111B-A541-4EA9-BB27-3244421F15B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9AB1111B-A541-4EA9-BB27-3244421F15B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -345,13 +345,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>57761</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>317988</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1279890</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>1234584</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -359,10 +359,10 @@
         <xdr:cNvPr id="6" name="Picture 5" descr="Rama">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D7D4049D-C68D-4FDB-A6EC-68C124016779}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{D7D4049D-C68D-4FDB-A6EC-68C124016779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -392,13 +392,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>48358</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1208942</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>1257300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -406,10 +406,10 @@
         <xdr:cNvPr id="7" name="Picture 6" descr="Mohan">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B05390-1331-4FAA-9153-45329DA2EA6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{21B05390-1331-4FAA-9153-45329DA2EA6C}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -439,13 +439,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>2</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1952626</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>1628775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -477,13 +477,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1866900</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>136546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -515,13 +515,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>303950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1952624</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>1054644</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -553,13 +553,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1952625</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>750694</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -591,13 +591,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1952625</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>752475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -628,19 +628,57 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1952625</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>752475</xdr:rowOff>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>61317</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="3.png"/>
+        <xdr:cNvPr id="16" name="Picture 15" descr="3.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7172325" y="190500"/>
+          <a:ext cx="1666875" cy="937617"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1924050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1076325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="3.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -653,46 +691,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7067550" y="12153900"/>
+          <a:off x="7038975" y="1390650"/>
           <a:ext cx="1952625" cy="752475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>174724</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1952625</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1273075</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="3.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7067550" y="13204924"/>
-          <a:ext cx="1952625" cy="1098351"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,7 +993,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1046,181 +1046,171 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="103.5" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" ht="69" customHeight="1">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="147" customHeight="1">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:10" ht="102" customHeight="1">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="215.25" customHeight="1">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:10" ht="103.5" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="150.75" customHeight="1">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" ht="147" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="84.75" customHeight="1">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" ht="215.25" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="99.75" customHeight="1">
+    <row r="7" spans="1:10" ht="150.75" customHeight="1">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="76.5" customHeight="1">
+    <row r="8" spans="1:10" ht="84.75" customHeight="1">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1228,28 +1218,28 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="64.5" customHeight="1">
+    <row r="9" spans="1:10" ht="99.75" customHeight="1">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1257,73 +1247,83 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="69" customHeight="1">
+    <row r="10" spans="1:10" ht="76.5" customHeight="1">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="F10" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="102" customHeight="1">
+    <row r="11" spans="1:10" ht="64.5" customHeight="1">
       <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added field department in tbl_examinations
</commit_message>
<xml_diff>
--- a/admin/uploads/excel.xlsx
+++ b/admin/uploads/excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Exam ID</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>Katmandu</t>
+  </si>
+  <si>
+    <t>EX_751153</t>
+  </si>
+  <si>
+    <t>Python version</t>
   </si>
 </sst>
 </file>
@@ -315,7 +321,7 @@
         <xdr:cNvPr id="5" name="Picture 4" descr="test image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9AB1111B-A541-4EA9-BB27-3244421F15B2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AB1111B-A541-4EA9-BB27-3244421F15B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -359,10 +365,10 @@
         <xdr:cNvPr id="6" name="Picture 5" descr="Rama">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{D7D4049D-C68D-4FDB-A6EC-68C124016779}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D7D4049D-C68D-4FDB-A6EC-68C124016779}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -406,10 +412,10 @@
         <xdr:cNvPr id="7" name="Picture 6" descr="Mohan">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{21B05390-1331-4FAA-9153-45329DA2EA6C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B05390-1331-4FAA-9153-45329DA2EA6C}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4AE8E70F-1419-4739-97B1-182C2E4A665D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -693,6 +699,44 @@
         <a:xfrm>
           <a:off x="7038975" y="1390650"/>
           <a:ext cx="1952625" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>164820</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1787805</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="3.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7232370" y="14325600"/>
+          <a:ext cx="1622985" cy="752475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,7 +1037,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1001,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1326,6 +1370,35 @@
         <v>28</v>
       </c>
     </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>